<commit_message>
Added course work SM
</commit_message>
<xml_diff>
--- a/System_Modeling/course_work_folder/assets/verification_T2.xlsx
+++ b/System_Modeling/course_work_folder/assets/verification_T2.xlsx
@@ -524,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D2" t="n">
         <v>50</v>
@@ -539,13 +539,13 @@
         <v>25</v>
       </c>
       <c r="H2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I2" t="n">
-        <v>59.76</v>
+        <v>59.88</v>
       </c>
       <c r="J2" t="n">
-        <v>29.76</v>
+        <v>29.88</v>
       </c>
       <c r="K2" t="n">
         <v>0.04</v>
@@ -554,16 +554,16 @@
         <v>10000</v>
       </c>
       <c r="M2" t="n">
-        <v>25446.23999999979</v>
+        <v>25533.12000000007</v>
       </c>
       <c r="N2" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0022</v>
+        <v>0.0019</v>
       </c>
       <c r="P2" t="n">
-        <v>0.04641</v>
+        <v>0.04008</v>
       </c>
     </row>
     <row r="3">
@@ -574,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="D3" t="n">
         <v>50</v>
@@ -589,13 +589,13 @@
         <v>25</v>
       </c>
       <c r="H3" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="I3" t="n">
-        <v>58.72</v>
+        <v>59.44</v>
       </c>
       <c r="J3" t="n">
-        <v>28.72</v>
+        <v>29.44</v>
       </c>
       <c r="K3" t="n">
         <v>0.04</v>
@@ -604,16 +604,16 @@
         <v>10000</v>
       </c>
       <c r="M3" t="n">
-        <v>25425.60000000011</v>
+        <v>25353.43999999983</v>
       </c>
       <c r="N3" t="n">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="O3" t="n">
         <v>0.0019</v>
       </c>
       <c r="P3" t="n">
-        <v>0.03958</v>
+        <v>0.03992</v>
       </c>
     </row>
     <row r="4">
@@ -624,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="D4" t="n">
         <v>50</v>
@@ -639,13 +639,13 @@
         <v>25</v>
       </c>
       <c r="H4" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I4" t="n">
-        <v>59.4</v>
+        <v>59.12</v>
       </c>
       <c r="J4" t="n">
-        <v>29.4</v>
+        <v>29.12</v>
       </c>
       <c r="K4" t="n">
         <v>0.04</v>
@@ -654,16 +654,16 @@
         <v>10000</v>
       </c>
       <c r="M4" t="n">
-        <v>25335.00000000017</v>
+        <v>25348.47999999993</v>
       </c>
       <c r="N4" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O4" t="n">
         <v>0.0019</v>
       </c>
       <c r="P4" t="n">
-        <v>0.04</v>
+        <v>0.03967</v>
       </c>
     </row>
     <row r="5">
@@ -674,7 +674,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="D5" t="n">
         <v>50</v>
@@ -689,13 +689,13 @@
         <v>25</v>
       </c>
       <c r="H5" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I5" t="n">
-        <v>58.64</v>
+        <v>59.04</v>
       </c>
       <c r="J5" t="n">
-        <v>28.64</v>
+        <v>29.04</v>
       </c>
       <c r="K5" t="n">
         <v>0.04</v>
@@ -704,16 +704,16 @@
         <v>10000</v>
       </c>
       <c r="M5" t="n">
-        <v>25301.27999999984</v>
+        <v>25252.08000000027</v>
       </c>
       <c r="N5" t="n">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0019</v>
+        <v>0.0021</v>
       </c>
       <c r="P5" t="n">
-        <v>0.03983</v>
+        <v>0.04403</v>
       </c>
     </row>
     <row r="6">
@@ -724,7 +724,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D6" t="n">
         <v>50</v>
@@ -739,13 +739,13 @@
         <v>25</v>
       </c>
       <c r="H6" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I6" t="n">
-        <v>59.52</v>
+        <v>59.72</v>
       </c>
       <c r="J6" t="n">
-        <v>29.52</v>
+        <v>29.72</v>
       </c>
       <c r="K6" t="n">
         <v>0.04</v>
@@ -754,16 +754,16 @@
         <v>10000</v>
       </c>
       <c r="M6" t="n">
-        <v>25243.92000000017</v>
+        <v>25247.84000000011</v>
       </c>
       <c r="N6" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="O6" t="n">
         <v>0.0019</v>
       </c>
       <c r="P6" t="n">
-        <v>0.04034</v>
+        <v>0.04025</v>
       </c>
     </row>
     <row r="7">
@@ -774,7 +774,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D7" t="n">
         <v>50</v>
@@ -789,13 +789,13 @@
         <v>25</v>
       </c>
       <c r="H7" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I7" t="n">
-        <v>59.56</v>
+        <v>59.8</v>
       </c>
       <c r="J7" t="n">
-        <v>29.56</v>
+        <v>29.8</v>
       </c>
       <c r="K7" t="n">
         <v>0.04</v>
@@ -804,16 +804,16 @@
         <v>10000</v>
       </c>
       <c r="M7" t="n">
-        <v>25233.64000000017</v>
+        <v>25225.99999999979</v>
       </c>
       <c r="N7" t="n">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0019</v>
+        <v>0.002</v>
       </c>
       <c r="P7" t="n">
-        <v>0.04051</v>
+        <v>0.04255</v>
       </c>
     </row>
     <row r="8">
@@ -824,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>400</v>
+        <v>432</v>
       </c>
       <c r="D8" t="n">
         <v>50</v>
@@ -839,13 +839,13 @@
         <v>25</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I8" t="n">
-        <v>60</v>
+        <v>58.72</v>
       </c>
       <c r="J8" t="n">
-        <v>30</v>
+        <v>28.72</v>
       </c>
       <c r="K8" t="n">
         <v>0.04</v>
@@ -854,16 +854,16 @@
         <v>10000</v>
       </c>
       <c r="M8" t="n">
-        <v>25230</v>
+        <v>25219.4400000001</v>
       </c>
       <c r="N8" t="n">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="O8" t="n">
         <v>0.002</v>
       </c>
       <c r="P8" t="n">
-        <v>0.04228</v>
+        <v>0.04193</v>
       </c>
     </row>
     <row r="9">
@@ -874,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>401</v>
+        <v>431</v>
       </c>
       <c r="D9" t="n">
         <v>50</v>
@@ -889,13 +889,13 @@
         <v>25</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="I9" t="n">
-        <v>59.96</v>
+        <v>58.76</v>
       </c>
       <c r="J9" t="n">
-        <v>29.96</v>
+        <v>28.76</v>
       </c>
       <c r="K9" t="n">
         <v>0.04</v>
@@ -904,16 +904,16 @@
         <v>10000</v>
       </c>
       <c r="M9" t="n">
-        <v>25181.39999999973</v>
+        <v>25207.27999999979</v>
       </c>
       <c r="N9" t="n">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="O9" t="n">
         <v>0.002</v>
       </c>
       <c r="P9" t="n">
-        <v>0.04301</v>
+        <v>0.04184</v>
       </c>
     </row>
     <row r="10">
@@ -924,7 +924,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="D10" t="n">
         <v>50</v>
@@ -939,13 +939,13 @@
         <v>25</v>
       </c>
       <c r="H10" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>59.12</v>
+        <v>59.96</v>
       </c>
       <c r="J10" t="n">
-        <v>29.12</v>
+        <v>29.96</v>
       </c>
       <c r="K10" t="n">
         <v>0.04</v>
@@ -954,16 +954,16 @@
         <v>10000</v>
       </c>
       <c r="M10" t="n">
-        <v>25171.99999999994</v>
+        <v>25181.27999999973</v>
       </c>
       <c r="N10" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O10" t="n">
-        <v>0.0019</v>
+        <v>0.002</v>
       </c>
       <c r="P10" t="n">
-        <v>0.04</v>
+        <v>0.04274</v>
       </c>
     </row>
     <row r="11">
@@ -974,7 +974,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>405</v>
+        <v>436</v>
       </c>
       <c r="D11" t="n">
         <v>50</v>
@@ -989,13 +989,13 @@
         <v>25</v>
       </c>
       <c r="H11" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="I11" t="n">
-        <v>59.8</v>
+        <v>58.56</v>
       </c>
       <c r="J11" t="n">
-        <v>29.8</v>
+        <v>28.56</v>
       </c>
       <c r="K11" t="n">
         <v>0.04</v>
@@ -1004,16 +1004,16 @@
         <v>10000</v>
       </c>
       <c r="M11" t="n">
-        <v>25166.39999999979</v>
+        <v>25147.44000000017</v>
       </c>
       <c r="N11" t="n">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="O11" t="n">
-        <v>0.0019</v>
+        <v>0.0018</v>
       </c>
       <c r="P11" t="n">
-        <v>0.0406</v>
+        <v>0.03797</v>
       </c>
     </row>
     <row r="12">
@@ -1024,7 +1024,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="D12" t="n">
         <v>50</v>
@@ -1039,13 +1039,13 @@
         <v>25</v>
       </c>
       <c r="H12" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I12" t="n">
-        <v>58.92</v>
+        <v>59.24</v>
       </c>
       <c r="J12" t="n">
-        <v>28.92</v>
+        <v>29.24</v>
       </c>
       <c r="K12" t="n">
         <v>0.04</v>
@@ -1054,16 +1054,16 @@
         <v>10000</v>
       </c>
       <c r="M12" t="n">
-        <v>25110.23999999974</v>
+        <v>25140.52000000021</v>
       </c>
       <c r="N12" t="n">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0018</v>
+        <v>0.002</v>
       </c>
       <c r="P12" t="n">
-        <v>0.03814</v>
+        <v>0.04228</v>
       </c>
     </row>
     <row r="13">
@@ -1074,7 +1074,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="D13" t="n">
         <v>50</v>
@@ -1089,13 +1089,13 @@
         <v>25</v>
       </c>
       <c r="H13" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I13" t="n">
-        <v>58.56</v>
+        <v>58.84</v>
       </c>
       <c r="J13" t="n">
-        <v>28.56</v>
+        <v>28.84</v>
       </c>
       <c r="K13" t="n">
         <v>0.04</v>
@@ -1104,16 +1104,16 @@
         <v>10000</v>
       </c>
       <c r="M13" t="n">
-        <v>25090.32000000016</v>
+        <v>25129.00000000006</v>
       </c>
       <c r="N13" t="n">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0019</v>
+        <v>0.0022</v>
       </c>
       <c r="P13" t="n">
-        <v>0.04025</v>
+        <v>0.04632</v>
       </c>
     </row>
     <row r="14">
@@ -1124,7 +1124,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D14" t="n">
         <v>50</v>
@@ -1139,13 +1139,13 @@
         <v>25</v>
       </c>
       <c r="H14" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I14" t="n">
-        <v>59.28</v>
+        <v>59.08</v>
       </c>
       <c r="J14" t="n">
-        <v>29.28</v>
+        <v>29.08</v>
       </c>
       <c r="K14" t="n">
         <v>0.04</v>
@@ -1154,16 +1154,16 @@
         <v>10000</v>
       </c>
       <c r="M14" t="n">
-        <v>25070.1599999999</v>
+        <v>25123.00000000027</v>
       </c>
       <c r="N14" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O14" t="n">
         <v>0.0019</v>
       </c>
       <c r="P14" t="n">
-        <v>0.04025</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="15">
@@ -1174,7 +1174,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="D15" t="n">
         <v>50</v>
@@ -1189,13 +1189,13 @@
         <v>25</v>
       </c>
       <c r="H15" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I15" t="n">
-        <v>59.48</v>
+        <v>59.76</v>
       </c>
       <c r="J15" t="n">
-        <v>29.48</v>
+        <v>29.76</v>
       </c>
       <c r="K15" t="n">
         <v>0.04</v>
@@ -1204,16 +1204,16 @@
         <v>10000</v>
       </c>
       <c r="M15" t="n">
-        <v>25045.59999999983</v>
+        <v>25117.4399999998</v>
       </c>
       <c r="N15" t="n">
         <v>97</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0019</v>
+        <v>0.002</v>
       </c>
       <c r="P15" t="n">
-        <v>0.04043</v>
+        <v>0.04264</v>
       </c>
     </row>
     <row r="16">
@@ -1224,7 +1224,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D16" t="n">
         <v>50</v>
@@ -1239,13 +1239,13 @@
         <v>25</v>
       </c>
       <c r="H16" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I16" t="n">
-        <v>58.28</v>
+        <v>58.2</v>
       </c>
       <c r="J16" t="n">
-        <v>28.28</v>
+        <v>28.2</v>
       </c>
       <c r="K16" t="n">
         <v>0.04</v>
@@ -1254,10 +1254,10 @@
         <v>10000</v>
       </c>
       <c r="M16" t="n">
-        <v>25036.1199999999</v>
+        <v>25087.80000000021</v>
       </c>
       <c r="N16" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O16" t="n">
         <v>0.0018</v>
@@ -1304,16 +1304,16 @@
         <v>10000</v>
       </c>
       <c r="M17" t="n">
-        <v>25034.80000000006</v>
+        <v>25064.64000000006</v>
       </c>
       <c r="N17" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O17" t="n">
         <v>0.002</v>
       </c>
       <c r="P17" t="n">
-        <v>0.04255</v>
+        <v>0.04246</v>
       </c>
     </row>
     <row r="18">
@@ -1324,7 +1324,7 @@
         <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>403</v>
+        <v>425</v>
       </c>
       <c r="D18" t="n">
         <v>50</v>
@@ -1339,13 +1339,13 @@
         <v>25</v>
       </c>
       <c r="H18" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="I18" t="n">
-        <v>59.88</v>
+        <v>59</v>
       </c>
       <c r="J18" t="n">
-        <v>29.88</v>
+        <v>29</v>
       </c>
       <c r="K18" t="n">
         <v>0.04</v>
@@ -1354,16 +1354,16 @@
         <v>10000</v>
       </c>
       <c r="M18" t="n">
-        <v>25024.20000000006</v>
+        <v>25027</v>
       </c>
       <c r="N18" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0021</v>
+        <v>0.0018</v>
       </c>
       <c r="P18" t="n">
-        <v>0.04516</v>
+        <v>0.03805</v>
       </c>
     </row>
     <row r="19">
@@ -1374,7 +1374,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D19" t="n">
         <v>50</v>
@@ -1389,13 +1389,13 @@
         <v>25</v>
       </c>
       <c r="H19" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I19" t="n">
-        <v>58.2</v>
+        <v>58.36</v>
       </c>
       <c r="J19" t="n">
-        <v>28.2</v>
+        <v>28.36</v>
       </c>
       <c r="K19" t="n">
         <v>0.04</v>
@@ -1404,16 +1404,16 @@
         <v>10000</v>
       </c>
       <c r="M19" t="n">
-        <v>24915.00000000021</v>
+        <v>25021.00000000016</v>
       </c>
       <c r="N19" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0018</v>
+        <v>0.0019</v>
       </c>
       <c r="P19" t="n">
-        <v>0.03789</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20">
@@ -1424,7 +1424,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="n">
-        <v>425</v>
+        <v>400</v>
       </c>
       <c r="D20" t="n">
         <v>50</v>
@@ -1439,13 +1439,13 @@
         <v>25</v>
       </c>
       <c r="H20" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J20" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K20" t="n">
         <v>0.04</v>
@@ -1454,16 +1454,16 @@
         <v>10000</v>
       </c>
       <c r="M20" t="n">
-        <v>24880</v>
+        <v>25020</v>
       </c>
       <c r="N20" t="n">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="O20" t="n">
-        <v>0.002</v>
+        <v>0.0023</v>
       </c>
       <c r="P20" t="n">
-        <v>0.04255</v>
+        <v>0.04894</v>
       </c>
     </row>
     <row r="21">
@@ -1474,7 +1474,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="n">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="D21" t="n">
         <v>50</v>
@@ -1489,13 +1489,13 @@
         <v>25</v>
       </c>
       <c r="H21" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I21" t="n">
-        <v>58.88</v>
+        <v>58.6</v>
       </c>
       <c r="J21" t="n">
-        <v>28.88</v>
+        <v>28.6</v>
       </c>
       <c r="K21" t="n">
         <v>0.04</v>
@@ -1504,16 +1504,16 @@
         <v>10000</v>
       </c>
       <c r="M21" t="n">
-        <v>24878.00000000006</v>
+        <v>25017.79999999984</v>
       </c>
       <c r="N21" t="n">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0019</v>
+        <v>0.0018</v>
       </c>
       <c r="P21" t="n">
-        <v>0.04</v>
+        <v>0.03805</v>
       </c>
     </row>
     <row r="22">
@@ -1524,7 +1524,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="n">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D22" t="n">
         <v>50</v>
@@ -1539,13 +1539,13 @@
         <v>25</v>
       </c>
       <c r="H22" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I22" t="n">
-        <v>58.6</v>
+        <v>58.88</v>
       </c>
       <c r="J22" t="n">
-        <v>28.6</v>
+        <v>28.88</v>
       </c>
       <c r="K22" t="n">
         <v>0.04</v>
@@ -1554,16 +1554,16 @@
         <v>10000</v>
       </c>
       <c r="M22" t="n">
-        <v>24867.79999999984</v>
+        <v>24972.48000000006</v>
       </c>
       <c r="N22" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O22" t="n">
-        <v>0.002</v>
+        <v>0.0019</v>
       </c>
       <c r="P22" t="n">
-        <v>0.04228</v>
+        <v>0.04034</v>
       </c>
     </row>
     <row r="23">
@@ -1574,7 +1574,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="n">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D23" t="n">
         <v>50</v>
@@ -1589,13 +1589,13 @@
         <v>25</v>
       </c>
       <c r="H23" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I23" t="n">
-        <v>59.6</v>
+        <v>59.56</v>
       </c>
       <c r="J23" t="n">
-        <v>29.6</v>
+        <v>29.56</v>
       </c>
       <c r="K23" t="n">
         <v>0.04</v>
@@ -1604,16 +1604,16 @@
         <v>10000</v>
       </c>
       <c r="M23" t="n">
-        <v>24863.59999999985</v>
+        <v>24962.76000000016</v>
       </c>
       <c r="N23" t="n">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0021</v>
+        <v>0.0019</v>
       </c>
       <c r="P23" t="n">
-        <v>0.04506</v>
+        <v>0.04034</v>
       </c>
     </row>
     <row r="24">
@@ -1624,7 +1624,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="n">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D24" t="n">
         <v>50</v>
@@ -1639,13 +1639,13 @@
         <v>25</v>
       </c>
       <c r="H24" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I24" t="n">
-        <v>58.96</v>
+        <v>58.8</v>
       </c>
       <c r="J24" t="n">
-        <v>28.96</v>
+        <v>28.8</v>
       </c>
       <c r="K24" t="n">
         <v>0.04</v>
@@ -1654,16 +1654,16 @@
         <v>10000</v>
       </c>
       <c r="M24" t="n">
-        <v>24862.23999999973</v>
+        <v>24961.19999999979</v>
       </c>
       <c r="N24" t="n">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="O24" t="n">
         <v>0.0018</v>
       </c>
       <c r="P24" t="n">
-        <v>0.03838</v>
+        <v>0.03797</v>
       </c>
     </row>
     <row r="25">
@@ -1674,7 +1674,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="n">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="D25" t="n">
         <v>50</v>
@@ -1689,13 +1689,13 @@
         <v>25</v>
       </c>
       <c r="H25" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="I25" t="n">
-        <v>59.08</v>
+        <v>59.92</v>
       </c>
       <c r="J25" t="n">
-        <v>29.08</v>
+        <v>29.92</v>
       </c>
       <c r="K25" t="n">
         <v>0.04</v>
@@ -1704,7 +1704,7 @@
         <v>10000</v>
       </c>
       <c r="M25" t="n">
-        <v>24856.68000000026</v>
+        <v>24952.71999999974</v>
       </c>
       <c r="N25" t="n">
         <v>99</v>
@@ -1713,7 +1713,7 @@
         <v>0.0019</v>
       </c>
       <c r="P25" t="n">
-        <v>0.04034</v>
+        <v>0.04077</v>
       </c>
     </row>
     <row r="26">
@@ -1724,7 +1724,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="n">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="D26" t="n">
         <v>50</v>
@@ -1739,13 +1739,13 @@
         <v>25</v>
       </c>
       <c r="H26" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I26" t="n">
-        <v>58.68</v>
+        <v>58.48</v>
       </c>
       <c r="J26" t="n">
-        <v>28.68</v>
+        <v>28.48</v>
       </c>
       <c r="K26" t="n">
         <v>0.04</v>
@@ -1754,16 +1754,16 @@
         <v>10000</v>
       </c>
       <c r="M26" t="n">
-        <v>24850.92000000011</v>
+        <v>24927.99999999983</v>
       </c>
       <c r="N26" t="n">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="O26" t="n">
         <v>0.0018</v>
       </c>
       <c r="P26" t="n">
-        <v>0.03838</v>
+        <v>0.03789</v>
       </c>
     </row>
     <row r="27">
@@ -1774,7 +1774,7 @@
         <v>8</v>
       </c>
       <c r="C27" t="n">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D27" t="n">
         <v>50</v>
@@ -1789,13 +1789,13 @@
         <v>25</v>
       </c>
       <c r="H27" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I27" t="n">
-        <v>58.36</v>
+        <v>58.52</v>
       </c>
       <c r="J27" t="n">
-        <v>28.36</v>
+        <v>28.52</v>
       </c>
       <c r="K27" t="n">
         <v>0.04</v>
@@ -1804,16 +1804,16 @@
         <v>10000</v>
       </c>
       <c r="M27" t="n">
-        <v>24841.00000000016</v>
+        <v>24918.48000000017</v>
       </c>
       <c r="N27" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O27" t="n">
         <v>0.0018</v>
       </c>
       <c r="P27" t="n">
-        <v>0.03789</v>
+        <v>0.03797</v>
       </c>
     </row>
     <row r="28">
@@ -1824,7 +1824,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="n">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D28" t="n">
         <v>50</v>
@@ -1839,13 +1839,13 @@
         <v>25</v>
       </c>
       <c r="H28" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I28" t="n">
-        <v>58.16</v>
+        <v>58</v>
       </c>
       <c r="J28" t="n">
-        <v>28.16</v>
+        <v>28</v>
       </c>
       <c r="K28" t="n">
         <v>0.04</v>
@@ -1854,16 +1854,16 @@
         <v>10000</v>
       </c>
       <c r="M28" t="n">
-        <v>24809.67999999994</v>
+        <v>24856</v>
       </c>
       <c r="N28" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="O28" t="n">
         <v>0.0018</v>
       </c>
       <c r="P28" t="n">
-        <v>0.03805</v>
+        <v>0.03814</v>
       </c>
     </row>
     <row r="29">
@@ -1874,7 +1874,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="n">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="D29" t="n">
         <v>50</v>
@@ -1889,13 +1889,13 @@
         <v>25</v>
       </c>
       <c r="H29" t="n">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I29" t="n">
-        <v>58.4</v>
+        <v>58.04</v>
       </c>
       <c r="J29" t="n">
-        <v>28.4</v>
+        <v>28.04</v>
       </c>
       <c r="K29" t="n">
         <v>0.04</v>
@@ -1904,16 +1904,16 @@
         <v>10000</v>
       </c>
       <c r="M29" t="n">
-        <v>24803.20000000015</v>
+        <v>24833.12000000028</v>
       </c>
       <c r="N29" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="O29" t="n">
         <v>0.0018</v>
       </c>
       <c r="P29" t="n">
-        <v>0.03805</v>
+        <v>0.03766</v>
       </c>
     </row>
     <row r="30">
@@ -1924,7 +1924,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D30" t="n">
         <v>50</v>
@@ -1939,13 +1939,13 @@
         <v>25</v>
       </c>
       <c r="H30" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I30" t="n">
-        <v>59.24</v>
+        <v>59.48</v>
       </c>
       <c r="J30" t="n">
-        <v>29.24</v>
+        <v>29.48</v>
       </c>
       <c r="K30" t="n">
         <v>0.04</v>
@@ -1954,16 +1954,16 @@
         <v>10000</v>
       </c>
       <c r="M30" t="n">
-        <v>24785.8400000002</v>
+        <v>24809.23999999983</v>
       </c>
       <c r="N30" t="n">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O30" t="n">
-        <v>0.0019</v>
+        <v>0.002</v>
       </c>
       <c r="P30" t="n">
-        <v>0.04077</v>
+        <v>0.0432</v>
       </c>
     </row>
     <row r="31">
@@ -1974,7 +1974,7 @@
         <v>8</v>
       </c>
       <c r="C31" t="n">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D31" t="n">
         <v>50</v>
@@ -1989,13 +1989,13 @@
         <v>25</v>
       </c>
       <c r="H31" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I31" t="n">
-        <v>59.36</v>
+        <v>59.32</v>
       </c>
       <c r="J31" t="n">
-        <v>29.36</v>
+        <v>29.32</v>
       </c>
       <c r="K31" t="n">
         <v>0.04</v>
@@ -2004,16 +2004,16 @@
         <v>10000</v>
       </c>
       <c r="M31" t="n">
-        <v>24780.48000000016</v>
+        <v>24795.15999999989</v>
       </c>
       <c r="N31" t="n">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="O31" t="n">
-        <v>0.002</v>
+        <v>0.0019</v>
       </c>
       <c r="P31" t="n">
-        <v>0.04274</v>
+        <v>0.04104</v>
       </c>
     </row>
     <row r="32">
@@ -2024,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="n">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="D32" t="n">
         <v>50</v>
@@ -2039,13 +2039,13 @@
         <v>25</v>
       </c>
       <c r="H32" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="I32" t="n">
-        <v>59.04</v>
+        <v>59.64</v>
       </c>
       <c r="J32" t="n">
-        <v>29.04</v>
+        <v>29.64</v>
       </c>
       <c r="K32" t="n">
         <v>0.04</v>
@@ -2054,16 +2054,16 @@
         <v>10000</v>
       </c>
       <c r="M32" t="n">
-        <v>24779.76000000027</v>
+        <v>24791.87999999984</v>
       </c>
       <c r="N32" t="n">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="O32" t="n">
-        <v>0.002</v>
+        <v>0.0019</v>
       </c>
       <c r="P32" t="n">
-        <v>0.04264</v>
+        <v>0.04069</v>
       </c>
     </row>
     <row r="33">
@@ -2074,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="n">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="D33" t="n">
         <v>50</v>
@@ -2089,13 +2089,13 @@
         <v>25</v>
       </c>
       <c r="H33" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I33" t="n">
-        <v>59.16</v>
+        <v>58.92</v>
       </c>
       <c r="J33" t="n">
-        <v>29.16</v>
+        <v>28.92</v>
       </c>
       <c r="K33" t="n">
         <v>0.04</v>
@@ -2104,16 +2104,16 @@
         <v>10000</v>
       </c>
       <c r="M33" t="n">
-        <v>24778.55999999994</v>
+        <v>24785.63999999974</v>
       </c>
       <c r="N33" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0019</v>
+        <v>0.0018</v>
       </c>
       <c r="P33" t="n">
-        <v>0.04077</v>
+        <v>0.03854</v>
       </c>
     </row>
     <row r="34">
@@ -2124,7 +2124,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="D34" t="n">
         <v>50</v>
@@ -2139,13 +2139,13 @@
         <v>25</v>
       </c>
       <c r="H34" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I34" t="n">
-        <v>59.92</v>
+        <v>59.52</v>
       </c>
       <c r="J34" t="n">
-        <v>29.92</v>
+        <v>29.52</v>
       </c>
       <c r="K34" t="n">
         <v>0.04</v>
@@ -2154,16 +2154,16 @@
         <v>10000</v>
       </c>
       <c r="M34" t="n">
-        <v>24772.95999999974</v>
+        <v>24766.80000000017</v>
       </c>
       <c r="N34" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O34" t="n">
-        <v>0.002</v>
+        <v>0.0021</v>
       </c>
       <c r="P34" t="n">
-        <v>0.0432</v>
+        <v>0.04516</v>
       </c>
     </row>
     <row r="35">
@@ -2174,7 +2174,7 @@
         <v>8</v>
       </c>
       <c r="C35" t="n">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D35" t="n">
         <v>50</v>
@@ -2189,13 +2189,13 @@
         <v>25</v>
       </c>
       <c r="H35" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I35" t="n">
-        <v>58.44</v>
+        <v>58.68</v>
       </c>
       <c r="J35" t="n">
-        <v>28.44</v>
+        <v>28.68</v>
       </c>
       <c r="K35" t="n">
         <v>0.04</v>
@@ -2204,16 +2204,16 @@
         <v>10000</v>
       </c>
       <c r="M35" t="n">
-        <v>24765.23999999985</v>
+        <v>24759.60000000011</v>
       </c>
       <c r="N35" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O35" t="n">
-        <v>0.002</v>
+        <v>0.0019</v>
       </c>
       <c r="P35" t="n">
-        <v>0.04246</v>
+        <v>0.04043</v>
       </c>
     </row>
     <row r="36">
@@ -2224,7 +2224,7 @@
         <v>8</v>
       </c>
       <c r="C36" t="n">
-        <v>430</v>
+        <v>446</v>
       </c>
       <c r="D36" t="n">
         <v>50</v>
@@ -2239,13 +2239,13 @@
         <v>25</v>
       </c>
       <c r="H36" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="I36" t="n">
-        <v>58.8</v>
+        <v>58.16</v>
       </c>
       <c r="J36" t="n">
-        <v>28.8</v>
+        <v>28.16</v>
       </c>
       <c r="K36" t="n">
         <v>0.04</v>
@@ -2254,16 +2254,16 @@
         <v>10000</v>
       </c>
       <c r="M36" t="n">
-        <v>24760.7999999998</v>
+        <v>24721.51999999994</v>
       </c>
       <c r="N36" t="n">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0019</v>
+        <v>0.0018</v>
       </c>
       <c r="P36" t="n">
-        <v>0.04077</v>
+        <v>0.03814</v>
       </c>
     </row>
     <row r="37">
@@ -2274,7 +2274,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="D37" t="n">
         <v>50</v>
@@ -2289,13 +2289,13 @@
         <v>25</v>
       </c>
       <c r="H37" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I37" t="n">
-        <v>59.44</v>
+        <v>59.28</v>
       </c>
       <c r="J37" t="n">
-        <v>29.44</v>
+        <v>29.28</v>
       </c>
       <c r="K37" t="n">
         <v>0.04</v>
@@ -2304,16 +2304,16 @@
         <v>10000</v>
       </c>
       <c r="M37" t="n">
-        <v>24758.47999999984</v>
+        <v>24714.4799999999</v>
       </c>
       <c r="N37" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O37" t="n">
         <v>0.0019</v>
       </c>
       <c r="P37" t="n">
-        <v>0.04069</v>
+        <v>0.04077</v>
       </c>
     </row>
     <row r="38">
@@ -2354,16 +2354,16 @@
         <v>10000</v>
       </c>
       <c r="M38" t="n">
-        <v>24708.8000000002</v>
+        <v>24647.2000000002</v>
       </c>
       <c r="N38" t="n">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="O38" t="n">
-        <v>0.0021</v>
+        <v>0.0019</v>
       </c>
       <c r="P38" t="n">
-        <v>0.04526</v>
+        <v>0.04077</v>
       </c>
     </row>
     <row r="39">
@@ -2374,7 +2374,7 @@
         <v>8</v>
       </c>
       <c r="C39" t="n">
-        <v>447</v>
+        <v>416</v>
       </c>
       <c r="D39" t="n">
         <v>50</v>
@@ -2389,13 +2389,13 @@
         <v>25</v>
       </c>
       <c r="H39" t="n">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="I39" t="n">
-        <v>58.12</v>
+        <v>59.36</v>
       </c>
       <c r="J39" t="n">
-        <v>28.12</v>
+        <v>29.36</v>
       </c>
       <c r="K39" t="n">
         <v>0.04</v>
@@ -2404,16 +2404,16 @@
         <v>10000</v>
       </c>
       <c r="M39" t="n">
-        <v>24702.63999999995</v>
+        <v>24633.04000000016</v>
       </c>
       <c r="N39" t="n">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="O39" t="n">
-        <v>0.0018</v>
+        <v>0.002</v>
       </c>
       <c r="P39" t="n">
-        <v>0.03814</v>
+        <v>0.0431</v>
       </c>
     </row>
     <row r="40">
@@ -2424,7 +2424,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>409</v>
+        <v>434</v>
       </c>
       <c r="D40" t="n">
         <v>50</v>
@@ -2439,13 +2439,13 @@
         <v>25</v>
       </c>
       <c r="H40" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="I40" t="n">
-        <v>59.64</v>
+        <v>58.64</v>
       </c>
       <c r="J40" t="n">
-        <v>29.64</v>
+        <v>28.64</v>
       </c>
       <c r="K40" t="n">
         <v>0.04</v>
@@ -2454,16 +2454,16 @@
         <v>10000</v>
       </c>
       <c r="M40" t="n">
-        <v>24614.03999999984</v>
+        <v>24590.79999999984</v>
       </c>
       <c r="N40" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O40" t="n">
-        <v>0.002</v>
+        <v>0.0018</v>
       </c>
       <c r="P40" t="n">
-        <v>0.04338</v>
+        <v>0.0383</v>
       </c>
     </row>
     <row r="41">
@@ -2474,7 +2474,7 @@
         <v>8</v>
       </c>
       <c r="C41" t="n">
-        <v>407</v>
+        <v>443</v>
       </c>
       <c r="D41" t="n">
         <v>50</v>
@@ -2489,13 +2489,13 @@
         <v>25</v>
       </c>
       <c r="H41" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="I41" t="n">
-        <v>59.72</v>
+        <v>58.28</v>
       </c>
       <c r="J41" t="n">
-        <v>29.72</v>
+        <v>28.28</v>
       </c>
       <c r="K41" t="n">
         <v>0.04</v>
@@ -2504,16 +2504,16 @@
         <v>10000</v>
       </c>
       <c r="M41" t="n">
-        <v>24590.92000000009</v>
+        <v>24571.59999999991</v>
       </c>
       <c r="N41" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="O41" t="n">
-        <v>0.0019</v>
+        <v>0.0018</v>
       </c>
       <c r="P41" t="n">
-        <v>0.04121</v>
+        <v>0.0383</v>
       </c>
     </row>
     <row r="42">
@@ -2524,7 +2524,7 @@
         <v>8</v>
       </c>
       <c r="C42" t="n">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="D42" t="n">
         <v>50</v>
@@ -2539,13 +2539,13 @@
         <v>25</v>
       </c>
       <c r="H42" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I42" t="n">
-        <v>58.76</v>
+        <v>59.16</v>
       </c>
       <c r="J42" t="n">
-        <v>28.76</v>
+        <v>29.16</v>
       </c>
       <c r="K42" t="n">
         <v>0.04</v>
@@ -2554,16 +2554,16 @@
         <v>10000</v>
       </c>
       <c r="M42" t="n">
-        <v>24590.91999999981</v>
+        <v>24511.07999999994</v>
       </c>
       <c r="N42" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O42" t="n">
-        <v>0.0019</v>
+        <v>0.002</v>
       </c>
       <c r="P42" t="n">
-        <v>0.04069</v>
+        <v>0.0432</v>
       </c>
     </row>
     <row r="43">
@@ -2574,7 +2574,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="n">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="D43" t="n">
         <v>50</v>
@@ -2589,13 +2589,13 @@
         <v>25</v>
       </c>
       <c r="H43" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I43" t="n">
-        <v>58.24</v>
+        <v>58.08</v>
       </c>
       <c r="J43" t="n">
-        <v>28.24</v>
+        <v>28.08</v>
       </c>
       <c r="K43" t="n">
         <v>0.04</v>
@@ -2604,16 +2604,16 @@
         <v>10000</v>
       </c>
       <c r="M43" t="n">
-        <v>24522.80000000019</v>
+        <v>24485.28000000025</v>
       </c>
       <c r="N43" t="n">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="O43" t="n">
         <v>0.0018</v>
       </c>
       <c r="P43" t="n">
-        <v>0.0383</v>
+        <v>0.03863</v>
       </c>
     </row>
     <row r="44">
@@ -2624,7 +2624,7 @@
         <v>8</v>
       </c>
       <c r="C44" t="n">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="D44" t="n">
         <v>50</v>
@@ -2639,13 +2639,13 @@
         <v>25</v>
       </c>
       <c r="H44" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I44" t="n">
-        <v>58</v>
+        <v>58.4</v>
       </c>
       <c r="J44" t="n">
-        <v>28</v>
+        <v>28.4</v>
       </c>
       <c r="K44" t="n">
         <v>0.04</v>
@@ -2654,16 +2654,16 @@
         <v>10000</v>
       </c>
       <c r="M44" t="n">
-        <v>24476</v>
+        <v>24481.20000000015</v>
       </c>
       <c r="N44" t="n">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="O44" t="n">
         <v>0.0018</v>
       </c>
       <c r="P44" t="n">
-        <v>0.03854</v>
+        <v>0.03846</v>
       </c>
     </row>
     <row r="45">
@@ -2674,7 +2674,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="n">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="D45" t="n">
         <v>50</v>
@@ -2689,13 +2689,13 @@
         <v>25</v>
       </c>
       <c r="H45" t="n">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="I45" t="n">
-        <v>58.32</v>
+        <v>58.96</v>
       </c>
       <c r="J45" t="n">
-        <v>28.32</v>
+        <v>28.96</v>
       </c>
       <c r="K45" t="n">
         <v>0.04</v>
@@ -2704,16 +2704,16 @@
         <v>10000</v>
       </c>
       <c r="M45" t="n">
-        <v>24422.15999999989</v>
+        <v>24417.43999999974</v>
       </c>
       <c r="N45" t="n">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="O45" t="n">
-        <v>0.0018</v>
+        <v>0.002</v>
       </c>
       <c r="P45" t="n">
-        <v>0.03888</v>
+        <v>0.0431</v>
       </c>
     </row>
     <row r="46">
@@ -2724,7 +2724,7 @@
         <v>8</v>
       </c>
       <c r="C46" t="n">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="D46" t="n">
         <v>50</v>
@@ -2739,13 +2739,13 @@
         <v>25</v>
       </c>
       <c r="H46" t="n">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="I46" t="n">
-        <v>58.84</v>
+        <v>59.68</v>
       </c>
       <c r="J46" t="n">
-        <v>28.84</v>
+        <v>29.68</v>
       </c>
       <c r="K46" t="n">
         <v>0.04</v>
@@ -2754,16 +2754,16 @@
         <v>10000</v>
       </c>
       <c r="M46" t="n">
-        <v>24396.40000000006</v>
+        <v>24393.7600000001</v>
       </c>
       <c r="N46" t="n">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="O46" t="n">
         <v>0.0019</v>
       </c>
       <c r="P46" t="n">
-        <v>0.0413</v>
+        <v>0.04158</v>
       </c>
     </row>
     <row r="47">
@@ -2774,7 +2774,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="n">
-        <v>417</v>
+        <v>442</v>
       </c>
       <c r="D47" t="n">
         <v>50</v>
@@ -2789,13 +2789,13 @@
         <v>25</v>
       </c>
       <c r="H47" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="I47" t="n">
-        <v>59.32</v>
+        <v>58.32</v>
       </c>
       <c r="J47" t="n">
-        <v>29.32</v>
+        <v>28.32</v>
       </c>
       <c r="K47" t="n">
         <v>0.04</v>
@@ -2804,16 +2804,16 @@
         <v>10000</v>
       </c>
       <c r="M47" t="n">
-        <v>24377.8799999999</v>
+        <v>24358.79999999989</v>
       </c>
       <c r="N47" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O47" t="n">
-        <v>0.0021</v>
+        <v>0.0018</v>
       </c>
       <c r="P47" t="n">
-        <v>0.04575</v>
+        <v>0.03871</v>
       </c>
     </row>
     <row r="48">
@@ -2824,7 +2824,7 @@
         <v>8</v>
       </c>
       <c r="C48" t="n">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D48" t="n">
         <v>50</v>
@@ -2839,13 +2839,13 @@
         <v>25</v>
       </c>
       <c r="H48" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I48" t="n">
-        <v>59.68</v>
+        <v>59.6</v>
       </c>
       <c r="J48" t="n">
-        <v>29.68</v>
+        <v>29.6</v>
       </c>
       <c r="K48" t="n">
         <v>0.04</v>
@@ -2854,16 +2854,16 @@
         <v>10000</v>
       </c>
       <c r="M48" t="n">
-        <v>24363.4400000001</v>
+        <v>24327.99999999986</v>
       </c>
       <c r="N48" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="O48" t="n">
-        <v>0.002</v>
+        <v>0.0019</v>
       </c>
       <c r="P48" t="n">
-        <v>0.04367</v>
+        <v>0.04176</v>
       </c>
     </row>
     <row r="49">
@@ -2874,7 +2874,7 @@
         <v>8</v>
       </c>
       <c r="C49" t="n">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="D49" t="n">
         <v>50</v>
@@ -2889,13 +2889,13 @@
         <v>25</v>
       </c>
       <c r="H49" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="I49" t="n">
-        <v>58.48</v>
+        <v>59.4</v>
       </c>
       <c r="J49" t="n">
-        <v>28.48</v>
+        <v>29.4</v>
       </c>
       <c r="K49" t="n">
         <v>0.04</v>
@@ -2904,16 +2904,16 @@
         <v>10000</v>
       </c>
       <c r="M49" t="n">
-        <v>24340.15999999983</v>
+        <v>24235.80000000013</v>
       </c>
       <c r="N49" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O49" t="n">
-        <v>0.0018</v>
+        <v>0.0019</v>
       </c>
       <c r="P49" t="n">
-        <v>0.03854</v>
+        <v>0.04158</v>
       </c>
     </row>
     <row r="50">
@@ -2924,7 +2924,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="n">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="D50" t="n">
         <v>50</v>
@@ -2939,13 +2939,13 @@
         <v>25</v>
       </c>
       <c r="H50" t="n">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I50" t="n">
-        <v>58.08</v>
+        <v>58.44</v>
       </c>
       <c r="J50" t="n">
-        <v>28.08</v>
+        <v>28.44</v>
       </c>
       <c r="K50" t="n">
         <v>0.04</v>
@@ -2954,16 +2954,16 @@
         <v>10000</v>
       </c>
       <c r="M50" t="n">
-        <v>24307.20000000024</v>
+        <v>24213.95999999986</v>
       </c>
       <c r="N50" t="n">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O50" t="n">
-        <v>0.0019</v>
+        <v>0.0018</v>
       </c>
       <c r="P50" t="n">
-        <v>0.04086</v>
+        <v>0.03922</v>
       </c>
     </row>
     <row r="51">
@@ -2974,7 +2974,7 @@
         <v>8</v>
       </c>
       <c r="C51" t="n">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="D51" t="n">
         <v>50</v>
@@ -2989,13 +2989,13 @@
         <v>25</v>
       </c>
       <c r="H51" t="n">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I51" t="n">
-        <v>58.52</v>
+        <v>58.24</v>
       </c>
       <c r="J51" t="n">
-        <v>28.52</v>
+        <v>28.24</v>
       </c>
       <c r="K51" t="n">
         <v>0.04</v>
@@ -3004,16 +3004,16 @@
         <v>10000</v>
       </c>
       <c r="M51" t="n">
-        <v>24129.20000000016</v>
+        <v>24213.92000000018</v>
       </c>
       <c r="N51" t="n">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="O51" t="n">
         <v>0.0019</v>
       </c>
       <c r="P51" t="n">
-        <v>0.0413</v>
+        <v>0.04148</v>
       </c>
     </row>
     <row r="52">
@@ -3024,7 +3024,7 @@
         <v>8</v>
       </c>
       <c r="C52" t="n">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D52" t="n">
         <v>50</v>
@@ -3039,13 +3039,13 @@
         <v>25</v>
       </c>
       <c r="H52" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I52" t="n">
-        <v>58.04</v>
+        <v>58.12</v>
       </c>
       <c r="J52" t="n">
-        <v>28.04</v>
+        <v>28.12</v>
       </c>
       <c r="K52" t="n">
         <v>0.04</v>
@@ -3054,16 +3054,16 @@
         <v>10000</v>
       </c>
       <c r="M52" t="n">
-        <v>24110.56000000026</v>
+        <v>24177.67999999995</v>
       </c>
       <c r="N52" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O52" t="n">
-        <v>0.0018</v>
+        <v>0.002</v>
       </c>
       <c r="P52" t="n">
-        <v>0.03879</v>
+        <v>0.0431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>